<commit_message>
Add init message about car for TL
</commit_message>
<xml_diff>
--- a/TrafficManagement.xlsx
+++ b/TrafficManagement.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -415,7 +415,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,18 +524,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -554,8 +555,14 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -574,8 +581,14 @@
       <c r="F2">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -594,8 +607,14 @@
       <c r="F3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -614,8 +633,14 @@
       <c r="F4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -634,8 +659,15 @@
       <c r="F5">
         <v>50</v>
       </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate if TL area is intersected, add activity messages saving
</commit_message>
<xml_diff>
--- a/TrafficManagement.xlsx
+++ b/TrafficManagement.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="TrafficLights" sheetId="1" r:id="rId1"/>
-    <sheet name="Cars" sheetId="2" r:id="rId2"/>
+    <sheet name="Cars (2)" sheetId="4" r:id="rId1"/>
+    <sheet name="TrafficLights" sheetId="1" r:id="rId2"/>
+    <sheet name="Cars" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -412,10 +413,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,12 +673,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H5" sqref="A3:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -605,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G3">
         <v>10</v>

</xml_diff>